<commit_message>
Changed paths of code to be compatible for all os
</commit_message>
<xml_diff>
--- a/General_Results/Pi_Chart_regions_results.xlsx
+++ b/General_Results/Pi_Chart_regions_results.xlsx
@@ -1,49 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklose\Documents\Python Scripts\MaTrace-Repo\MaTrace-Copper\General_Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8016" windowWidth="14808" xWindow="240" yWindow="108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Pi_charts" sheetId="2" r:id="rId2"/>
-    <sheet name="Regional_losses" sheetId="3" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pi_charts" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Regional_losses" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,26 +46,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -360,43 +356,693 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B2:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BAU</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>EPRreuse</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>All_amb</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>20.77782416756113</v>
+      </c>
+      <c r="P5" t="n">
+        <v>21.02556480491424</v>
+      </c>
+      <c r="R5" t="n">
+        <v>20.77138811585175</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n">
+        <v>33.04300530202713</v>
+      </c>
+      <c r="P6" t="n">
+        <v>35.96210539096652</v>
+      </c>
+      <c r="R6" t="n">
+        <v>27.7626493963804</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n">
+        <v>392.6631664180442</v>
+      </c>
+      <c r="P7" t="n">
+        <v>181.5754647695708</v>
+      </c>
+      <c r="R7" t="n">
+        <v>194.7362715075931</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n">
+        <v>19.76837060289324</v>
+      </c>
+      <c r="P8" t="n">
+        <v>24.83996057545004</v>
+      </c>
+      <c r="R8" t="n">
+        <v>25.25410119983471</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>473.1167399952967</v>
+      </c>
+      <c r="P9" t="n">
+        <v>515.7987458935493</v>
+      </c>
+      <c r="R9" t="n">
+        <v>261.9164805424659</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>1273.718103270524</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1427.366395786021</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1693.462345574268</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BAU</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>EPRreuse</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>All_amb</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>19.7812253842597</v>
+      </c>
+      <c r="P14" t="n">
+        <v>19.84967925796809</v>
+      </c>
+      <c r="R14" t="n">
+        <v>19.73169689503435</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
+        <v>344.842864800689</v>
+      </c>
+      <c r="P15" t="n">
+        <v>391.7250659560598</v>
+      </c>
+      <c r="R15" t="n">
+        <v>202.7334321290823</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="n">
+        <v>1440.42166486934</v>
+      </c>
+      <c r="P16" t="n">
+        <v>763.2528463620415</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1080.794137653233</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="n">
+        <v>304.7096603793004</v>
+      </c>
+      <c r="P17" t="n">
+        <v>83.44881235676111</v>
+      </c>
+      <c r="R17" t="n">
+        <v>90.78620387750506</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>4085.059427373394</v>
+      </c>
+      <c r="P18" t="n">
+        <v>4491.617902773238</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1611.421425665387</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>4011.123669407094</v>
+      </c>
+      <c r="P19" t="n">
+        <v>4537.531596376302</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7279.910735271014</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BAU</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>EPRreuse</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>All_amb</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>1.169378291102058</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1.166852129868285</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1.151547248150494</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>13.56780151585428</v>
+      </c>
+      <c r="P24" t="n">
+        <v>15.02625991904589</v>
+      </c>
+      <c r="R24" t="n">
+        <v>2.980942810170696</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>59.85327503301331</v>
+      </c>
+      <c r="P25" t="n">
+        <v>35.10805621951775</v>
+      </c>
+      <c r="R25" t="n">
+        <v>31.67432288506629</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>148.3667460281561</v>
+      </c>
+      <c r="P26" t="n">
+        <v>125.0051197624631</v>
+      </c>
+      <c r="R26" t="n">
+        <v>4.121736990329867</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>52.29887335140297</v>
+      </c>
+      <c r="P27" t="n">
+        <v>53.48110437217215</v>
+      </c>
+      <c r="R27" t="n">
+        <v>40.63611932258286</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>390.0534984195283</v>
+      </c>
+      <c r="P28" t="n">
+        <v>427.3872627715195</v>
+      </c>
+      <c r="R28" t="n">
+        <v>551.2768854727558</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BAU</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>EPRreuse</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>All_amb</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NAM</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>NAM</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>NAM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>12.76717516237608</v>
+      </c>
+      <c r="P32" t="n">
+        <v>12.90807280837683</v>
+      </c>
+      <c r="R32" t="n">
+        <v>12.86494534993547</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>26.49675629397487</v>
+      </c>
+      <c r="P33" t="n">
+        <v>28.11715024419879</v>
+      </c>
+      <c r="R33" t="n">
+        <v>22.63259603003617</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>339.5078061232531</v>
+      </c>
+      <c r="P34" t="n">
+        <v>180.6657785446415</v>
+      </c>
+      <c r="R34" t="n">
+        <v>200.9956775805312</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>15.59679152298207</v>
+      </c>
+      <c r="P35" t="n">
+        <v>19.89375651630913</v>
+      </c>
+      <c r="R35" t="n">
+        <v>20.81605313940318</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>320.7378487962864</v>
+      </c>
+      <c r="P36" t="n">
+        <v>342.3920486559787</v>
+      </c>
+      <c r="R36" t="n">
+        <v>146.2726454112802</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>1244.120448245589</v>
+      </c>
+      <c r="P37" t="n">
+        <v>1372.843910735388</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1532.10883633772</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6195</v>
+      </c>
+      <c r="B4" t="n">
+        <v>152</v>
+      </c>
+      <c r="C4" t="n">
+        <v>715</v>
+      </c>
+      <c r="D4" t="n">
+        <v>939</v>
+      </c>
+      <c r="E4" t="n">
+        <v>356</v>
+      </c>
+      <c r="F4" t="n">
+        <v>241</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1228</v>
+      </c>
+      <c r="H4" t="n">
+        <v>275</v>
+      </c>
+      <c r="I4" t="n">
+        <v>529</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9109.833536171765</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>5750</v>
+      </c>
+      <c r="B32" t="n">
+        <v>128</v>
+      </c>
+      <c r="C32" t="n">
+        <v>584</v>
+      </c>
+      <c r="D32" t="n">
+        <v>779</v>
+      </c>
+      <c r="E32" t="n">
+        <v>349</v>
+      </c>
+      <c r="F32" t="n">
+        <v>218</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1002</v>
+      </c>
+      <c r="H32" t="n">
+        <v>230</v>
+      </c>
+      <c r="I32" t="n">
+        <v>454</v>
+      </c>
+      <c r="M32" t="n">
+        <v>10236.18837706896</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3005</v>
+      </c>
+      <c r="B36" t="n">
+        <v>99</v>
+      </c>
+      <c r="C36" t="n">
+        <v>404</v>
+      </c>
+      <c r="D36" t="n">
+        <v>530</v>
+      </c>
+      <c r="E36" t="n">
+        <v>292</v>
+      </c>
+      <c r="F36" t="n">
+        <v>117</v>
+      </c>
+      <c r="G36" t="n">
+        <v>626</v>
+      </c>
+      <c r="H36" t="n">
+        <v>81</v>
+      </c>
+      <c r="I36" t="n">
+        <v>180</v>
+      </c>
+      <c r="M36" t="n">
+        <v>14384.3374662432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>